<commit_message>
added plugin to read xlsx and post to server side
authUtil to get user instead of hardcoding
Auditable does preInsert and preUpdate
trim word before insertion
</commit_message>
<xml_diff>
--- a/docs/tcm-words.xlsx
+++ b/docs/tcm-words.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="732">
   <si>
     <t>热因热用</t>
   </si>
@@ -2582,7 +2582,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D1" sqref="D1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2744,10 +2744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2830,65 +2830,57 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B10" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B11" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B12" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B13" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B14" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B15" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B16" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>716</v>
-      </c>
-      <c r="B17" t="s">
         <v>731</v>
       </c>
     </row>

</xml_diff>